<commit_message>
add github links and favicons
</commit_message>
<xml_diff>
--- a/excel/Calculating TC temp.xlsx
+++ b/excel/Calculating TC temp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovino/PythonGit/webapps/epic-tc-calculator/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47CC06BD-A434-414D-9421-B5A4FD50EC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EDEFD4-7342-E341-82C5-C22AD08F17D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="26240" windowHeight="16420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="26240" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First_TC shield" sheetId="1" r:id="rId1"/>
@@ -290,50 +290,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>y = 3.7129E-02x</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> - 2.9693E+00x</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> + 5.4464E+01x + 6.5414E+02</t>
-    </r>
-  </si>
-  <si>
     <t>Max temperature</t>
   </si>
   <si>
@@ -427,6 +383,45 @@
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve"> + 1.2367E+02x + 4.6354E+02</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>y = 3.7129E-02x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> - 2.9693E+00x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> + 5.4464E+01x + 6.5414E+02</t>
     </r>
   </si>
 </sst>
@@ -3069,8 +3064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3131,22 +3126,22 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B6" s="4">
-        <v>2.4E-2</v>
+        <v>0.02</v>
       </c>
       <c r="C6" s="5">
-        <v>0.32200000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" ref="D6:E6" si="0">B6*25.4</f>
-        <v>0.60960000000000003</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" si="0"/>
-        <v>8.178799999999999</v>
+        <v>7.6199999999999992</v>
       </c>
       <c r="F6" s="6">
         <f>(E6/2)+(D6*0.756)</f>
-        <v>4.5502575999999992</v>
+        <v>4.1940479999999996</v>
       </c>
       <c r="G6" s="7">
         <f>((0.037129*(11.76922856
@@ -3156,7 +3151,7 @@
 ^3))-(2.9693*((11.76922856-F6)
 ^2))+(54.464*(11.76922856-F6)
 )+654.14)</f>
-        <v>37.834119431046474</v>
+        <v>31.909771004660684</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -3209,26 +3204,26 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B11" s="4">
-        <v>2.4E-2</v>
+        <v>0.02</v>
       </c>
       <c r="C11" s="5">
-        <v>0.32200000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" ref="D11:E11" si="1">B11*25.4</f>
-        <v>0.60960000000000003</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="E11" s="6">
         <f t="shared" si="1"/>
-        <v>8.178799999999999</v>
+        <v>7.6199999999999992</v>
       </c>
       <c r="F11" s="6">
         <f>(E11/2)+(D11*0.756)</f>
-        <v>4.5502575999999992</v>
+        <v>4.1940479999999996</v>
       </c>
       <c r="G11" s="7">
         <f>((-0.013609*(11.2807309644187)^4) + (0.60653*(11.2807309644187)^3) + (-12.281*(11.2807309644187)^2) + (123.67*11.2807309644187) + (463.54)) - ((-0.013609*((11.2807309644187-F11))^4) + (0.60653*((11.2807309644187-F11))^3) + (-12.281*((11.2807309644187-F11))^2) + (123.67*(11.2807309644187-F11)) + (463.54))</f>
-        <v>49.546552653828712</v>
+        <v>41.394506105901883</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4224,7 +4219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0"/>
+    <sheetView zoomScale="132" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6231,7 +6228,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6359,7 +6356,7 @@
         <v>928.09903754942741</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="16" x14ac:dyDescent="0.2">
@@ -6370,7 +6367,7 @@
         <v>931.49001070168731</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="16" x14ac:dyDescent="0.2">
@@ -6381,10 +6378,10 @@
         <v>937.41421417452818</v>
       </c>
       <c r="H18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="17" t="s">
         <v>25</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="16" x14ac:dyDescent="0.2">
@@ -7793,8 +7790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7868,7 +7865,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
@@ -8354,8 +8351,8 @@
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
-      <c r="H18" s="6" t="s">
-        <v>28</v>
+      <c r="H18" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
@@ -8389,7 +8386,7 @@
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
       <c r="H19" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
@@ -8422,10 +8419,10 @@
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
       <c r="H20" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="17" t="s">
         <v>25</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>26</v>
       </c>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>

</xml_diff>